<commit_message>
Actualizados PDF y Excel
</commit_message>
<xml_diff>
--- a/sdi1920-entrega1-605-614/docs/sdi1920-entrega1-605-614.xlsx
+++ b/sdi1920-entrega1-605-614/docs/sdi1920-entrega1-605-614.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UO265081\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D22EFCD-72CD-4B3C-9BF7-4919C8529175}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{867F88AA-5C5B-42C8-AC11-BA6D33BB2466}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="48">
   <si>
     <t>Puntuación (Para rellenar por el profesor)</t>
   </si>
@@ -228,12 +228,18 @@
   <si>
     <t>Se comprueba que el archivo es una imagen (se aceptan formatos .png, .jpg y .jpeg)</t>
   </si>
+  <si>
+    <t>Participación</t>
+  </si>
+  <si>
+    <t>50%-50%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +283,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -298,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -559,11 +571,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -592,7 +619,74 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -600,72 +694,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84:G96"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -960,100 +993,106 @@
     <col min="7" max="7" width="39.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-    </row>
-    <row r="4" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="46">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="25">
         <f>G31</f>
         <v>11</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-    </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="I4" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:8" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="46">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25">
         <f>G44</f>
         <v>0</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-    </row>
-    <row r="7" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="44" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="29">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="28">
         <f>A4-A6</f>
         <v>11</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="30" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
-    </row>
-    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1077,7 +1116,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1105,7 +1144,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -1133,7 +1172,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1161,7 +1200,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -1605,28 +1644,28 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="5" t="s">
         <v>17</v>
       </c>
@@ -1635,110 +1674,110 @@
       <c r="A34" s="6">
         <v>1</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>2</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>3</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>4</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>5</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>6</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>7</v>
       </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
       <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>8</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
       <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>9</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>10</v>
       </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
@@ -1777,15 +1816,15 @@
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="38"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="34"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -1800,11 +1839,11 @@
       <c r="D48" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E48" s="27" t="s">
+      <c r="E48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -1819,11 +1858,11 @@
       <c r="D49" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E49" s="20" t="s">
+      <c r="E49" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -1838,9 +1877,9 @@
       <c r="D50" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -1855,9 +1894,9 @@
       <c r="D51" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E51" s="20"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
@@ -1872,9 +1911,9 @@
       <c r="D52" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -1889,9 +1928,9 @@
       <c r="D53" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E53" s="20"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
@@ -1906,9 +1945,9 @@
       <c r="D54" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E54" s="20"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
@@ -1923,9 +1962,9 @@
       <c r="D55" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E55" s="20"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
@@ -1940,9 +1979,9 @@
       <c r="D56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E56" s="20"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
@@ -1957,9 +1996,9 @@
       <c r="D57" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E57" s="20"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
@@ -1974,9 +2013,9 @@
       <c r="D58" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E58" s="20"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -1991,9 +2030,9 @@
       <c r="D59" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E59" s="20"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -2008,9 +2047,9 @@
       <c r="D60" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="24"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="26"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="43"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -2025,9 +2064,9 @@
       <c r="D61" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E61" s="20"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -2042,9 +2081,9 @@
       <c r="D62" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E62" s="20"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -2059,9 +2098,9 @@
       <c r="D63" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E63" s="20"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
@@ -2076,9 +2115,9 @@
       <c r="D64" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E64" s="20"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -2093,9 +2132,9 @@
       <c r="D65" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E65" s="20"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="21"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -2110,9 +2149,9 @@
       <c r="D66" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E66" s="20"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
@@ -2127,9 +2166,9 @@
       <c r="D67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E67" s="20"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="44"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -2144,9 +2183,9 @@
       <c r="D68" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E68" s="20"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="44"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -2161,9 +2200,9 @@
       <c r="D69" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E69" s="20"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="44"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
@@ -2178,9 +2217,9 @@
       <c r="D70" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E70" s="20"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -2195,9 +2234,9 @@
       <c r="D71" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E71" s="20"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
@@ -2212,9 +2251,9 @@
       <c r="D72" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E72" s="22"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="23"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="46"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -2229,9 +2268,9 @@
       <c r="D73" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E73" s="20"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
@@ -2246,9 +2285,9 @@
       <c r="D74" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E74" s="20"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -2263,9 +2302,9 @@
       <c r="D75" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="20"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -2280,9 +2319,9 @@
       <c r="D76" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E76" s="20"/>
-      <c r="F76" s="21"/>
-      <c r="G76" s="21"/>
+      <c r="E76" s="38"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="44"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -2297,9 +2336,9 @@
       <c r="D77" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E77" s="20"/>
-      <c r="F77" s="21"/>
-      <c r="G77" s="21"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -2314,9 +2353,9 @@
       <c r="D78" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E78" s="20"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="21"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
@@ -2331,9 +2370,9 @@
       <c r="D79" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E79" s="20"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="44"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -2348,9 +2387,9 @@
       <c r="D80" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E80" s="20"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
@@ -2365,9 +2404,9 @@
       <c r="D81" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E81" s="20"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
@@ -2382,9 +2421,9 @@
       <c r="D82" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E82" s="20"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="21"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="44"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
@@ -2399,9 +2438,9 @@
       <c r="D83" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E83" s="20"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
@@ -2416,11 +2455,11 @@
       <c r="D84" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E84" s="20" t="s">
+      <c r="E84" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
@@ -2435,11 +2474,11 @@
       <c r="D85" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E85" s="20" t="s">
+      <c r="E85" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
@@ -2452,9 +2491,9 @@
       <c r="D86" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E86" s="20"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
@@ -2467,9 +2506,9 @@
       <c r="D87" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E87" s="20"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
@@ -2482,9 +2521,9 @@
       <c r="D88" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E88" s="20"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
@@ -2497,9 +2536,9 @@
       <c r="D89" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E89" s="20"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="21"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -2512,9 +2551,9 @@
       <c r="D90" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E90" s="20"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="21"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
@@ -2527,9 +2566,9 @@
       <c r="D91" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E91" s="20"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="21"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="44"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
@@ -2542,9 +2581,9 @@
       <c r="D92" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E92" s="20"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="21"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
@@ -2557,9 +2596,9 @@
       <c r="D93" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E93" s="20"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="21"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
@@ -2572,9 +2611,9 @@
       <c r="D94" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E94" s="20"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="21"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="44"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
@@ -2587,9 +2626,9 @@
       <c r="D95" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E95" s="20"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="21"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="44"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
@@ -2602,18 +2641,60 @@
       <c r="D96" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E96" s="20"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="21"/>
+      <c r="E96" s="38"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="E86:G86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="E89:G89"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="E84:G84"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A11:G11"/>
@@ -2630,54 +2711,12 @@
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="B43:F43"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E84:G84"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="E86:G86"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="E89:G89"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>